<commit_message>
Added start of record layout
</commit_message>
<xml_diff>
--- a/_book/offline/assets/sync-1a.xlsx
+++ b/_book/offline/assets/sync-1a.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="10260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="10260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>Conflict detected?</t>
   </si>
@@ -112,6 +113,24 @@
   </si>
   <si>
     <t>Resulting record</t>
+  </si>
+  <si>
+    <t>Input to conflict resolver:</t>
+  </si>
+  <si>
+    <t>Conflict resolver's choices:</t>
+  </si>
+  <si>
+    <t>Use remote service's current record</t>
+  </si>
+  <si>
+    <t>Use client service's proposed record</t>
+  </si>
+  <si>
+    <t>Use business rules to determine result</t>
+  </si>
+  <si>
+    <t>123 Fifth Ave.</t>
   </si>
 </sst>
 </file>
@@ -135,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,8 +183,14 @@
         </stop>
       </gradientFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -205,6 +230,19 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="dotted">
         <color indexed="64"/>
       </right>
@@ -345,38 +383,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -807,75 +896,147 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D8"/>
+  <dimension ref="B2:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="25" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="D3" s="25"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="25"/>
+      <c r="D4" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F4" s="22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="25" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="25"/>
+      <c r="D6" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E6" s="23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="25"/>
+      <c r="D7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E7" s="23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="25"/>
+      <c r="D8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E8" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F8" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="25"/>
+      <c r="D9" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F9" s="22" t="s">
         <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="4.140625" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>